<commit_message>
Test sur les requêtes par rapport aux listes
</commit_message>
<xml_diff>
--- a/Documentation/TEST/FicheTestHippie.xlsx
+++ b/Documentation/TEST/FicheTestHippie.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="129">
   <si>
     <t>Test No.</t>
   </si>
@@ -383,12 +383,90 @@
   <si>
     <t>Modifie le champ marchandise_statut à `"Réservé" et rafraichi la liste</t>
   </si>
+  <si>
+    <t>GOOGLE MAPS / RÉSULTATS DES REQUÊTES</t>
+  </si>
+  <si>
+    <t>Liste marchandises disponible</t>
+  </si>
+  <si>
+    <t>Liste de marchandise sisponible par entreprise</t>
+  </si>
+  <si>
+    <t>Sur le onClick de l'icône Liste marchandises disponible de la carte</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Devrait retourner le nombre d'enregistrements contenu dans la base de données </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>alimentaire</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dont le marchandise_statut est à disponible</t>
+    </r>
+  </si>
+  <si>
+    <t>Après avoir sélectionné une enttreprise sur la carte, faire afficher la liste des dons de cette entreprise</t>
+  </si>
+  <si>
+    <t>Devrait afficher les marchandises disponible de l'entreprise sélectionnée</t>
+  </si>
+  <si>
+    <t>Bouton  MES RÉSERVATIONS</t>
+  </si>
+  <si>
+    <t>Sur le onClick du bouton  MES RÉSERVATIONS</t>
+  </si>
+  <si>
+    <t>Devrait afficher la liste des marchadises réservées par l'organisme connecté</t>
+  </si>
+  <si>
+    <t>Retourne les 2 enregistrements dont le marchandise_statut est à "Réservé"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Retourne les 9 enregistrements  dont le marchandise_statut est à "Disponible" de la base de données </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>alimentaire</t>
+    </r>
+  </si>
+  <si>
+    <t>N'affiche rien</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="dd\-mm\-yy;@"/>
+  </numFmts>
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -456,6 +534,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -465,7 +551,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="27">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -807,12 +893,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="3"/>
+      </right>
+      <top style="thin">
+        <color theme="3"/>
+      </top>
+      <bottom style="thin">
+        <color theme="3"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -937,18 +1036,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -976,18 +1069,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1016,6 +1097,51 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1048,8 +1174,8 @@
     <xdr:to>
       <xdr:col>1</xdr:col>
       <xdr:colOff>274988</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>676274</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>865</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1372,19 +1498,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H104"/>
+  <dimension ref="A1:H92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="A71" sqref="A71:XFD71"/>
+      <selection pane="bottomLeft" activeCell="B79" sqref="B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.5703125" style="8" customWidth="1"/>
     <col min="2" max="2" width="17.140625" style="9" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" style="9" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" style="9" customWidth="1"/>
     <col min="5" max="5" width="39.42578125" style="9" customWidth="1"/>
     <col min="6" max="6" width="39.42578125" style="8" customWidth="1"/>
@@ -1394,13 +1520,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="55" t="s">
+      <c r="C1" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="55"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="55"/>
-      <c r="G1" s="55"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -1419,7 +1545,7 @@
       </c>
       <c r="B4" s="11">
         <f ca="1">TODAY()</f>
-        <v>42395</v>
+        <v>42401</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1455,16 +1581,16 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="63" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="57"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="58"/>
+      <c r="B9" s="64"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="65"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
@@ -1831,16 +1957,16 @@
       <c r="H30" s="17"/>
     </row>
     <row r="31" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="57"/>
-      <c r="C31" s="57"/>
-      <c r="D31" s="57"/>
-      <c r="E31" s="57"/>
-      <c r="F31" s="57"/>
-      <c r="G31" s="57"/>
-      <c r="H31" s="58"/>
+      <c r="B31" s="64"/>
+      <c r="C31" s="64"/>
+      <c r="D31" s="64"/>
+      <c r="E31" s="64"/>
+      <c r="F31" s="64"/>
+      <c r="G31" s="64"/>
+      <c r="H31" s="65"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="18">
@@ -1999,16 +2125,16 @@
       <c r="H44" s="6"/>
     </row>
     <row r="45" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="56" t="s">
+      <c r="A45" s="63" t="s">
         <v>92</v>
       </c>
-      <c r="B45" s="57"/>
-      <c r="C45" s="57"/>
-      <c r="D45" s="57"/>
-      <c r="E45" s="57"/>
-      <c r="F45" s="57"/>
-      <c r="G45" s="57"/>
-      <c r="H45" s="58"/>
+      <c r="B45" s="64"/>
+      <c r="C45" s="64"/>
+      <c r="D45" s="64"/>
+      <c r="E45" s="64"/>
+      <c r="F45" s="64"/>
+      <c r="G45" s="64"/>
+      <c r="H45" s="65"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="18">
@@ -2032,7 +2158,9 @@
       <c r="G46" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="H46" s="34"/>
+      <c r="H46" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" s="18">
@@ -2056,7 +2184,9 @@
       <c r="G47" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="H47" s="35"/>
+      <c r="H47" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="18">
@@ -2078,7 +2208,9 @@
       <c r="G48" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="H48" s="35"/>
+      <c r="H48" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" s="18">
@@ -2102,7 +2234,9 @@
       <c r="G49" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="H49" s="35"/>
+      <c r="H49" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="18">
@@ -2126,7 +2260,9 @@
       <c r="G50" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="H50" s="35"/>
+      <c r="H50" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="18">
@@ -2150,7 +2286,9 @@
       <c r="G51" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="H51" s="35"/>
+      <c r="H51" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="18">
@@ -2172,7 +2310,9 @@
       <c r="G52" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="H52" s="42"/>
+      <c r="H52" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="18">
@@ -2196,7 +2336,9 @@
       <c r="G53" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H53" s="6"/>
+      <c r="H53" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="18">
@@ -2211,7 +2353,7 @@
       <c r="D54" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="E54" s="43" t="s">
+      <c r="E54" s="42" t="s">
         <v>52</v>
       </c>
       <c r="F54" s="27" t="s">
@@ -2220,7 +2362,9 @@
       <c r="G54" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H54" s="6"/>
+      <c r="H54" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" s="18">
@@ -2241,10 +2385,12 @@
       <c r="F55" s="27">
         <v>10.1</v>
       </c>
-      <c r="G55" s="44" t="s">
+      <c r="G55" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="H55" s="45"/>
+      <c r="H55" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" s="18">
@@ -2265,13 +2411,15 @@
       <c r="F56" s="27">
         <v>10.11</v>
       </c>
-      <c r="G56" s="44" t="s">
+      <c r="G56" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="H56" s="45"/>
+      <c r="H56" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="46">
+      <c r="A57" s="44">
         <v>46</v>
       </c>
       <c r="B57" s="41" t="s">
@@ -2289,8 +2437,10 @@
       <c r="F57" s="27">
         <v>10.11</v>
       </c>
-      <c r="G57" s="44"/>
-      <c r="H57" s="45"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" s="18">
@@ -2309,16 +2459,18 @@
       <c r="F58" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="G58" s="44" t="s">
+      <c r="G58" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="H58" s="45"/>
+      <c r="H58" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" s="18">
         <v>48</v>
       </c>
-      <c r="B59" s="49" t="s">
+      <c r="B59" s="47" t="s">
         <v>51</v>
       </c>
       <c r="C59" s="25">
@@ -2331,34 +2483,38 @@
       <c r="F59" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="G59" s="44" t="s">
+      <c r="G59" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="H59" s="45"/>
+      <c r="H59" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="60" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="18">
         <v>49</v>
       </c>
-      <c r="B60" s="50" t="s">
+      <c r="B60" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="C60" s="51">
+      <c r="C60" s="49">
         <v>11111111111</v>
       </c>
-      <c r="D60" s="51" t="s">
+      <c r="D60" s="49" t="s">
         <v>57</v>
       </c>
-      <c r="E60" s="52" t="s">
+      <c r="E60" s="50" t="s">
         <v>84</v>
       </c>
-      <c r="F60" s="53" t="s">
+      <c r="F60" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="G60" s="54" t="s">
+      <c r="G60" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="H60" s="45"/>
+      <c r="H60" s="73">
+        <v>42395</v>
+      </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" s="18">
@@ -2375,10 +2531,12 @@
       <c r="F61" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="G61" s="44" t="s">
+      <c r="G61" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="H61" s="45"/>
+      <c r="H61" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" s="18">
@@ -2397,10 +2555,12 @@
       <c r="F62" s="31" t="s">
         <v>76</v>
       </c>
-      <c r="G62" s="44" t="s">
+      <c r="G62" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="H62" s="45"/>
+      <c r="H62" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" s="18">
@@ -2421,10 +2581,12 @@
       <c r="F63" s="31" t="s">
         <v>75</v>
       </c>
-      <c r="G63" s="44" t="s">
+      <c r="G63" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="H63" s="45"/>
+      <c r="H63" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" s="18">
@@ -2442,13 +2604,15 @@
       <c r="E64" s="38" t="s">
         <v>65</v>
       </c>
-      <c r="F64" s="48" t="s">
+      <c r="F64" s="46" t="s">
         <v>80</v>
       </c>
       <c r="G64" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H64" s="17"/>
+      <c r="H64" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" s="18">
@@ -2466,13 +2630,15 @@
       <c r="E65" s="38" t="s">
         <v>88</v>
       </c>
-      <c r="F65" s="48" t="s">
+      <c r="F65" s="46" t="s">
         <v>89</v>
       </c>
       <c r="G65" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H65" s="17"/>
+      <c r="H65" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="66" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A66" s="18">
@@ -2486,13 +2652,15 @@
       <c r="E66" s="38" t="s">
         <v>67</v>
       </c>
-      <c r="F66" s="48" t="s">
+      <c r="F66" s="46" t="s">
         <v>73</v>
       </c>
       <c r="G66" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H66" s="17"/>
+      <c r="H66" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A67" s="18">
@@ -2506,13 +2674,15 @@
       <c r="E67" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="F67" s="48" t="s">
+      <c r="F67" s="46" t="s">
         <v>78</v>
       </c>
       <c r="G67" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H67" s="17"/>
+      <c r="H67" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A68" s="18">
@@ -2530,13 +2700,15 @@
       <c r="E68" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="F68" s="48" t="s">
+      <c r="F68" s="46" t="s">
         <v>79</v>
       </c>
       <c r="G68" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H68" s="17"/>
+      <c r="H68" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A69" s="18">
@@ -2546,19 +2718,21 @@
         <v>96</v>
       </c>
       <c r="C69" s="32"/>
-      <c r="D69" s="61" t="s">
+      <c r="D69" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="E69" s="59" t="s">
+      <c r="E69" s="53" t="s">
         <v>102</v>
       </c>
-      <c r="F69" s="60" t="s">
+      <c r="F69" s="54" t="s">
         <v>94</v>
       </c>
       <c r="G69" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="H69" s="34"/>
+      <c r="H69" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="23">
@@ -2580,415 +2754,335 @@
       <c r="G70" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="H70" s="37"/>
+      <c r="H70" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="71" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="56" t="s">
+      <c r="A71" s="63" t="s">
         <v>110</v>
       </c>
-      <c r="B71" s="57"/>
-      <c r="C71" s="57"/>
-      <c r="D71" s="57"/>
-      <c r="E71" s="57"/>
-      <c r="F71" s="57"/>
-      <c r="G71" s="57"/>
-      <c r="H71" s="58"/>
+      <c r="B71" s="64"/>
+      <c r="C71" s="64"/>
+      <c r="D71" s="64"/>
+      <c r="E71" s="64"/>
+      <c r="F71" s="64"/>
+      <c r="G71" s="64"/>
+      <c r="H71" s="65"/>
     </row>
     <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="18">
         <v>61</v>
       </c>
-      <c r="B72" s="59" t="s">
+      <c r="B72" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="C72" s="59"/>
-      <c r="D72" s="59" t="s">
+      <c r="C72" s="53"/>
+      <c r="D72" s="53" t="s">
         <v>106</v>
       </c>
-      <c r="E72" s="59" t="s">
+      <c r="E72" s="53" t="s">
         <v>103</v>
       </c>
-      <c r="F72" s="62" t="s">
+      <c r="F72" s="56" t="s">
         <v>107</v>
       </c>
-      <c r="G72" s="59" t="s">
+      <c r="G72" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="H72" s="63"/>
+      <c r="H72" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="73" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A73" s="18">
         <v>62</v>
       </c>
-      <c r="B73" s="59" t="s">
+      <c r="B73" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="C73" s="59"/>
-      <c r="D73" s="59" t="s">
+      <c r="C73" s="53"/>
+      <c r="D73" s="53" t="s">
         <v>105</v>
       </c>
-      <c r="E73" s="59" t="s">
+      <c r="E73" s="53" t="s">
         <v>113</v>
       </c>
-      <c r="F73" s="62" t="s">
+      <c r="F73" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="G73" s="59" t="s">
+      <c r="G73" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="H73" s="63"/>
+      <c r="H73" s="67">
+        <v>42395</v>
+      </c>
     </row>
     <row r="74" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A74" s="18">
         <v>63</v>
       </c>
-      <c r="B74" s="59" t="s">
+      <c r="B74" s="53" t="s">
         <v>111</v>
       </c>
-      <c r="C74" s="59"/>
-      <c r="D74" s="59" t="s">
+      <c r="C74" s="53"/>
+      <c r="D74" s="53" t="s">
         <v>112</v>
       </c>
-      <c r="E74" s="59" t="s">
+      <c r="E74" s="53" t="s">
         <v>114</v>
       </c>
-      <c r="F74" s="62" t="s">
+      <c r="F74" s="56" t="s">
         <v>115</v>
       </c>
-      <c r="G74" s="59"/>
-      <c r="H74" s="63"/>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" s="18">
+      <c r="G74" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="H74" s="67">
+        <v>42395</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="63" t="s">
+        <v>116</v>
+      </c>
+      <c r="B75" s="70"/>
+      <c r="C75" s="70"/>
+      <c r="D75" s="70"/>
+      <c r="E75" s="64"/>
+      <c r="F75" s="64"/>
+      <c r="G75" s="64"/>
+      <c r="H75" s="65"/>
+    </row>
+    <row r="76" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+      <c r="A76" s="44">
         <v>64</v>
       </c>
-      <c r="B75" s="43"/>
-      <c r="C75" s="43"/>
-      <c r="D75" s="43"/>
-      <c r="E75" s="43"/>
-      <c r="F75" s="64"/>
-      <c r="G75" s="43"/>
-      <c r="H75" s="65"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="18">
+      <c r="B76" s="38" t="s">
+        <v>117</v>
+      </c>
+      <c r="C76" s="38" t="s">
+        <v>119</v>
+      </c>
+      <c r="D76" s="38"/>
+      <c r="E76" s="69" t="s">
+        <v>120</v>
+      </c>
+      <c r="F76" s="71" t="s">
+        <v>127</v>
+      </c>
+      <c r="G76" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="H76" s="72">
+        <v>42401</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+      <c r="A77" s="18">
         <v>65</v>
       </c>
-      <c r="B76" s="29"/>
-      <c r="C76" s="29"/>
-      <c r="D76" s="29"/>
-      <c r="E76" s="29"/>
-      <c r="F76" s="29"/>
-      <c r="G76" s="38"/>
-      <c r="H76" s="38"/>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="18">
+      <c r="B77" s="74" t="s">
+        <v>118</v>
+      </c>
+      <c r="C77" s="74" t="s">
+        <v>121</v>
+      </c>
+      <c r="D77" s="74"/>
+      <c r="E77" s="75" t="s">
+        <v>122</v>
+      </c>
+      <c r="F77" s="76" t="s">
+        <v>128</v>
+      </c>
+      <c r="G77" s="75" t="s">
+        <v>91</v>
+      </c>
+      <c r="H77" s="77">
+        <v>42401</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A78" s="18">
         <v>66</v>
       </c>
-      <c r="B77" s="29"/>
-      <c r="C77" s="29"/>
-      <c r="D77" s="29"/>
-      <c r="E77" s="29"/>
-      <c r="F77" s="29"/>
-      <c r="G77" s="38"/>
-      <c r="H77" s="38"/>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="18">
-        <v>67</v>
-      </c>
-      <c r="B78" s="29"/>
-      <c r="C78" s="29"/>
-      <c r="D78" s="29"/>
-      <c r="E78" s="29"/>
-      <c r="F78" s="27"/>
-      <c r="G78" s="66"/>
-      <c r="H78" s="67"/>
+      <c r="B78" s="53" t="s">
+        <v>123</v>
+      </c>
+      <c r="C78" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="D78" s="53"/>
+      <c r="E78" s="53" t="s">
+        <v>125</v>
+      </c>
+      <c r="F78" s="56" t="s">
+        <v>126</v>
+      </c>
+      <c r="G78" s="53" t="s">
+        <v>74</v>
+      </c>
+      <c r="H78" s="72">
+        <v>42401</v>
+      </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="18">
-        <v>68</v>
-      </c>
-      <c r="B79" s="29"/>
-      <c r="C79" s="29"/>
-      <c r="D79" s="29"/>
-      <c r="E79" s="29"/>
-      <c r="F79" s="27"/>
-      <c r="G79" s="66"/>
-      <c r="H79" s="67"/>
+        <v>67</v>
+      </c>
+      <c r="B79" s="42"/>
+      <c r="C79" s="42"/>
+      <c r="D79" s="42"/>
+      <c r="E79" s="42"/>
+      <c r="F79" s="58"/>
+      <c r="G79" s="42"/>
+      <c r="H79" s="59"/>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" s="18">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B80" s="29"/>
       <c r="C80" s="29"/>
       <c r="D80" s="29"/>
       <c r="E80" s="29"/>
-      <c r="F80" s="27"/>
-      <c r="G80" s="66"/>
-      <c r="H80" s="67"/>
+      <c r="F80" s="29"/>
+      <c r="G80" s="38"/>
+      <c r="H80" s="38"/>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="18">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B81" s="29"/>
       <c r="C81" s="29"/>
       <c r="D81" s="29"/>
       <c r="E81" s="29"/>
-      <c r="F81" s="27"/>
-      <c r="G81" s="66"/>
-      <c r="H81" s="67"/>
+      <c r="F81" s="29"/>
+      <c r="G81" s="38"/>
+      <c r="H81" s="38"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" s="18">
-        <v>71</v>
-      </c>
-      <c r="B82" s="25"/>
-      <c r="C82" s="25"/>
-      <c r="D82" s="25"/>
+        <v>70</v>
+      </c>
+      <c r="B82" s="29"/>
+      <c r="C82" s="29"/>
+      <c r="D82" s="29"/>
       <c r="E82" s="29"/>
       <c r="F82" s="27"/>
-      <c r="G82" s="44"/>
-      <c r="H82" s="45"/>
+      <c r="G82" s="60"/>
+      <c r="H82" s="61"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" s="18">
-        <v>72</v>
-      </c>
-      <c r="B83" s="25"/>
-      <c r="C83" s="25"/>
-      <c r="D83" s="25"/>
+        <v>71</v>
+      </c>
+      <c r="B83" s="29"/>
+      <c r="C83" s="29"/>
+      <c r="D83" s="29"/>
       <c r="E83" s="29"/>
-      <c r="F83" s="30"/>
-      <c r="G83" s="44"/>
-      <c r="H83" s="45"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="18">
-        <v>73</v>
-      </c>
-      <c r="B84" s="25"/>
-      <c r="C84" s="25"/>
-      <c r="D84" s="25"/>
-      <c r="E84" s="29"/>
-      <c r="F84" s="27"/>
-      <c r="G84" s="44"/>
-      <c r="H84" s="45"/>
+      <c r="F83" s="27"/>
+      <c r="G83" s="60"/>
+      <c r="H83" s="61"/>
+    </row>
+    <row r="84" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="63" t="s">
+        <v>109</v>
+      </c>
+      <c r="B84" s="64"/>
+      <c r="C84" s="64"/>
+      <c r="D84" s="64"/>
+      <c r="E84" s="64"/>
+      <c r="F84" s="64"/>
+      <c r="G84" s="64"/>
+      <c r="H84" s="65"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="18">
-        <v>74</v>
-      </c>
-      <c r="B85" s="6"/>
-      <c r="C85" s="25"/>
-      <c r="D85" s="25"/>
-      <c r="E85" s="29"/>
-      <c r="F85" s="30"/>
-      <c r="G85" s="44"/>
-      <c r="H85" s="45"/>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="18">
-        <v>75</v>
-      </c>
-      <c r="B86" s="6"/>
-      <c r="C86" s="6"/>
-      <c r="D86" s="6"/>
-      <c r="E86" s="38"/>
-      <c r="F86" s="47"/>
-      <c r="G86" s="6"/>
-      <c r="H86" s="17"/>
-    </row>
-    <row r="87" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="56" t="s">
-        <v>109</v>
-      </c>
-      <c r="B87" s="57"/>
-      <c r="C87" s="57"/>
-      <c r="D87" s="57"/>
-      <c r="E87" s="57"/>
-      <c r="F87" s="57"/>
-      <c r="G87" s="57"/>
-      <c r="H87" s="58"/>
+      <c r="A85" s="18"/>
+      <c r="B85" s="53"/>
+      <c r="C85" s="53"/>
+      <c r="D85" s="53"/>
+      <c r="E85" s="53"/>
+      <c r="F85" s="56"/>
+      <c r="G85" s="53"/>
+      <c r="H85" s="57"/>
+    </row>
+    <row r="86" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="A86" s="18"/>
+      <c r="B86" s="53"/>
+      <c r="C86" s="62"/>
+      <c r="D86" s="53"/>
+      <c r="E86" s="53"/>
+      <c r="F86" s="56"/>
+      <c r="G86" s="53"/>
+      <c r="H86" s="57"/>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="18"/>
+      <c r="B87" s="53"/>
+      <c r="C87" s="53"/>
+      <c r="D87" s="53"/>
+      <c r="E87" s="53"/>
+      <c r="F87" s="56"/>
+      <c r="G87" s="53"/>
+      <c r="H87" s="57"/>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" s="18"/>
-      <c r="B88" s="59"/>
-      <c r="C88" s="59"/>
-      <c r="D88" s="59"/>
-      <c r="E88" s="59"/>
-      <c r="F88" s="62"/>
-      <c r="G88" s="59"/>
-      <c r="H88" s="63"/>
-    </row>
-    <row r="89" spans="1:8" ht="18" x14ac:dyDescent="0.25">
+      <c r="B88" s="42"/>
+      <c r="C88" s="42"/>
+      <c r="D88" s="42"/>
+      <c r="E88" s="42"/>
+      <c r="F88" s="58"/>
+      <c r="G88" s="42"/>
+      <c r="H88" s="59"/>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" s="18"/>
-      <c r="B89" s="59"/>
-      <c r="C89" s="68"/>
-      <c r="D89" s="59"/>
-      <c r="E89" s="59"/>
-      <c r="F89" s="62"/>
-      <c r="G89" s="59"/>
-      <c r="H89" s="63"/>
+      <c r="B89" s="29"/>
+      <c r="C89" s="29"/>
+      <c r="D89" s="29"/>
+      <c r="E89" s="29"/>
+      <c r="F89" s="29"/>
+      <c r="G89" s="38"/>
+      <c r="H89" s="38"/>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" s="18"/>
-      <c r="B90" s="59"/>
-      <c r="C90" s="59"/>
-      <c r="D90" s="59"/>
-      <c r="E90" s="59"/>
-      <c r="F90" s="62"/>
-      <c r="G90" s="59"/>
-      <c r="H90" s="63"/>
+      <c r="B90" s="29"/>
+      <c r="C90" s="29"/>
+      <c r="D90" s="29"/>
+      <c r="E90" s="29"/>
+      <c r="F90" s="29"/>
+      <c r="G90" s="38"/>
+      <c r="H90" s="38"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="18"/>
-      <c r="B91" s="43"/>
-      <c r="C91" s="43"/>
-      <c r="D91" s="43"/>
-      <c r="E91" s="43"/>
-      <c r="F91" s="64"/>
-      <c r="G91" s="43"/>
-      <c r="H91" s="65"/>
+      <c r="A91" s="23"/>
+      <c r="B91" s="29"/>
+      <c r="C91" s="29"/>
+      <c r="D91" s="29"/>
+      <c r="E91" s="29"/>
+      <c r="F91" s="27"/>
+      <c r="G91" s="60"/>
+      <c r="H91" s="61"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="18"/>
-      <c r="B92" s="29"/>
-      <c r="C92" s="29"/>
-      <c r="D92" s="29"/>
-      <c r="E92" s="29"/>
-      <c r="F92" s="29"/>
+      <c r="A92" s="6"/>
+      <c r="B92" s="38"/>
+      <c r="C92" s="38"/>
+      <c r="D92" s="38"/>
+      <c r="E92" s="38"/>
+      <c r="F92" s="45"/>
       <c r="G92" s="38"/>
-      <c r="H92" s="38"/>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="18"/>
-      <c r="B93" s="29"/>
-      <c r="C93" s="29"/>
-      <c r="D93" s="29"/>
-      <c r="E93" s="29"/>
-      <c r="F93" s="29"/>
-      <c r="G93" s="38"/>
-      <c r="H93" s="38"/>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" s="18"/>
-      <c r="B94" s="29"/>
-      <c r="C94" s="29"/>
-      <c r="D94" s="29"/>
-      <c r="E94" s="29"/>
-      <c r="F94" s="27"/>
-      <c r="G94" s="66"/>
-      <c r="H94" s="67"/>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" s="18"/>
-      <c r="B95" s="29"/>
-      <c r="C95" s="29"/>
-      <c r="D95" s="29"/>
-      <c r="E95" s="29"/>
-      <c r="F95" s="27"/>
-      <c r="G95" s="66"/>
-      <c r="H95" s="67"/>
-    </row>
-    <row r="96" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A96" s="56"/>
-      <c r="B96" s="57"/>
-      <c r="C96" s="57"/>
-      <c r="D96" s="57"/>
-      <c r="E96" s="57"/>
-      <c r="F96" s="57"/>
-      <c r="G96" s="57"/>
-      <c r="H96" s="58"/>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" s="18"/>
-      <c r="B97" s="59"/>
-      <c r="C97" s="59"/>
-      <c r="D97" s="59"/>
-      <c r="E97" s="59"/>
-      <c r="F97" s="62"/>
-      <c r="G97" s="59"/>
-      <c r="H97" s="63"/>
-    </row>
-    <row r="98" spans="1:8" ht="18" x14ac:dyDescent="0.25">
-      <c r="A98" s="18"/>
-      <c r="B98" s="59"/>
-      <c r="C98" s="68"/>
-      <c r="D98" s="59"/>
-      <c r="E98" s="59"/>
-      <c r="F98" s="62"/>
-      <c r="G98" s="59"/>
-      <c r="H98" s="63"/>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" s="18"/>
-      <c r="B99" s="59"/>
-      <c r="C99" s="59"/>
-      <c r="D99" s="59"/>
-      <c r="E99" s="59"/>
-      <c r="F99" s="62"/>
-      <c r="G99" s="59"/>
-      <c r="H99" s="63"/>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" s="18"/>
-      <c r="B100" s="43"/>
-      <c r="C100" s="43"/>
-      <c r="D100" s="43"/>
-      <c r="E100" s="43"/>
-      <c r="F100" s="64"/>
-      <c r="G100" s="43"/>
-      <c r="H100" s="65"/>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" s="18"/>
-      <c r="B101" s="29"/>
-      <c r="C101" s="29"/>
-      <c r="D101" s="29"/>
-      <c r="E101" s="29"/>
-      <c r="F101" s="29"/>
-      <c r="G101" s="38"/>
-      <c r="H101" s="38"/>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" s="18"/>
-      <c r="B102" s="29"/>
-      <c r="C102" s="29"/>
-      <c r="D102" s="29"/>
-      <c r="E102" s="29"/>
-      <c r="F102" s="29"/>
-      <c r="G102" s="38"/>
-      <c r="H102" s="38"/>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" s="18"/>
-      <c r="B103" s="29"/>
-      <c r="C103" s="29"/>
-      <c r="D103" s="29"/>
-      <c r="E103" s="29"/>
-      <c r="F103" s="27"/>
-      <c r="G103" s="66"/>
-      <c r="H103" s="67"/>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" s="18"/>
-      <c r="B104" s="29"/>
-      <c r="C104" s="29"/>
-      <c r="D104" s="29"/>
-      <c r="E104" s="29"/>
-      <c r="F104" s="27"/>
-      <c r="G104" s="66"/>
-      <c r="H104" s="67"/>
+      <c r="H92" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A71:H71"/>
-    <mergeCell ref="A87:H87"/>
-    <mergeCell ref="A96:H96"/>
+    <mergeCell ref="A75:H75"/>
+    <mergeCell ref="A84:H84"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="A9:H9"/>
     <mergeCell ref="A31:H31"/>

</xml_diff>

<commit_message>
Petits ajouts, sur les tests
</commit_message>
<xml_diff>
--- a/Documentation/TEST/FicheTestHippie.xlsx
+++ b/Documentation/TEST/FicheTestHippie.xlsx
@@ -428,9 +428,6 @@
     <t>Devrait afficher les marchandises disponible de l'entreprise sélectionnée</t>
   </si>
   <si>
-    <t>Bouton  MES RÉSERVATIONS</t>
-  </si>
-  <si>
     <t>Sur le onClick du bouton  MES RÉSERVATIONS</t>
   </si>
   <si>
@@ -458,13 +455,16 @@
   <si>
     <t>N'affiche rien</t>
   </si>
+  <si>
+    <t>Bouton  MES RÉSERVATIONS (Liste de mes réservations)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="dd\-mm\-yy;@"/>
+    <numFmt numFmtId="164" formatCode="dd\-mm\-yy;@"/>
   </numFmts>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
@@ -1099,19 +1099,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
@@ -1120,16 +1108,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1143,6 +1128,21 @@
     </xf>
     <xf numFmtId="14" fontId="4" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1501,9 +1501,9 @@
   <dimension ref="A1:H92"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B4" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="B79" sqref="B79"/>
+      <selection pane="bottomLeft" activeCell="B78" sqref="B78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1520,13 +1520,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="53.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C1" s="66" t="s">
+      <c r="C1" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="66"/>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
@@ -1545,7 +1545,7 @@
       </c>
       <c r="B4" s="11">
         <f ca="1">TODAY()</f>
-        <v>42401</v>
+        <v>42402</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1581,16 +1581,16 @@
       </c>
     </row>
     <row r="9" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="63" t="s">
+      <c r="A9" s="73" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="64"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="65"/>
+      <c r="B9" s="74"/>
+      <c r="C9" s="74"/>
+      <c r="D9" s="74"/>
+      <c r="E9" s="74"/>
+      <c r="F9" s="74"/>
+      <c r="G9" s="74"/>
+      <c r="H9" s="75"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="13">
@@ -1957,16 +1957,16 @@
       <c r="H30" s="17"/>
     </row>
     <row r="31" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="63" t="s">
+      <c r="A31" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="B31" s="64"/>
-      <c r="C31" s="64"/>
-      <c r="D31" s="64"/>
-      <c r="E31" s="64"/>
-      <c r="F31" s="64"/>
-      <c r="G31" s="64"/>
-      <c r="H31" s="65"/>
+      <c r="B31" s="74"/>
+      <c r="C31" s="74"/>
+      <c r="D31" s="74"/>
+      <c r="E31" s="74"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="74"/>
+      <c r="H31" s="75"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="18">
@@ -2125,16 +2125,16 @@
       <c r="H44" s="6"/>
     </row>
     <row r="45" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="63" t="s">
+      <c r="A45" s="73" t="s">
         <v>92</v>
       </c>
-      <c r="B45" s="64"/>
-      <c r="C45" s="64"/>
-      <c r="D45" s="64"/>
-      <c r="E45" s="64"/>
-      <c r="F45" s="64"/>
-      <c r="G45" s="64"/>
-      <c r="H45" s="65"/>
+      <c r="B45" s="74"/>
+      <c r="C45" s="74"/>
+      <c r="D45" s="74"/>
+      <c r="E45" s="74"/>
+      <c r="F45" s="74"/>
+      <c r="G45" s="74"/>
+      <c r="H45" s="75"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="18">
@@ -2158,7 +2158,7 @@
       <c r="G46" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="H46" s="67">
+      <c r="H46" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2184,7 +2184,7 @@
       <c r="G47" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="H47" s="67">
+      <c r="H47" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2208,7 +2208,7 @@
       <c r="G48" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="H48" s="67">
+      <c r="H48" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2234,7 +2234,7 @@
       <c r="G49" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="H49" s="67">
+      <c r="H49" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2260,7 +2260,7 @@
       <c r="G50" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="H50" s="67">
+      <c r="H50" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2286,7 +2286,7 @@
       <c r="G51" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="H51" s="67">
+      <c r="H51" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2310,7 +2310,7 @@
       <c r="G52" s="41" t="s">
         <v>74</v>
       </c>
-      <c r="H52" s="67">
+      <c r="H52" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2336,7 +2336,7 @@
       <c r="G53" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H53" s="67">
+      <c r="H53" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2362,7 +2362,7 @@
       <c r="G54" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H54" s="67">
+      <c r="H54" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2388,7 +2388,7 @@
       <c r="G55" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="H55" s="67">
+      <c r="H55" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2414,7 +2414,7 @@
       <c r="G56" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="H56" s="67">
+      <c r="H56" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2438,7 +2438,7 @@
         <v>10.11</v>
       </c>
       <c r="G57" s="43"/>
-      <c r="H57" s="67">
+      <c r="H57" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2462,7 +2462,7 @@
       <c r="G58" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="H58" s="67">
+      <c r="H58" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2486,7 +2486,7 @@
       <c r="G59" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="H59" s="67">
+      <c r="H59" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2512,7 +2512,7 @@
       <c r="G60" s="52" t="s">
         <v>91</v>
       </c>
-      <c r="H60" s="73">
+      <c r="H60" s="68">
         <v>42395</v>
       </c>
     </row>
@@ -2534,7 +2534,7 @@
       <c r="G61" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="H61" s="67">
+      <c r="H61" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2558,7 +2558,7 @@
       <c r="G62" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="H62" s="67">
+      <c r="H62" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2584,7 +2584,7 @@
       <c r="G63" s="43" t="s">
         <v>74</v>
       </c>
-      <c r="H63" s="67">
+      <c r="H63" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2610,7 +2610,7 @@
       <c r="G64" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H64" s="67">
+      <c r="H64" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2636,7 +2636,7 @@
       <c r="G65" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H65" s="67">
+      <c r="H65" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2658,7 +2658,7 @@
       <c r="G66" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H66" s="67">
+      <c r="H66" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2680,7 +2680,7 @@
       <c r="G67" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H67" s="67">
+      <c r="H67" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2706,7 +2706,7 @@
       <c r="G68" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="H68" s="67">
+      <c r="H68" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2730,7 +2730,7 @@
       <c r="G69" s="32" t="s">
         <v>74</v>
       </c>
-      <c r="H69" s="67">
+      <c r="H69" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2754,21 +2754,21 @@
       <c r="G70" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="H70" s="67">
+      <c r="H70" s="63">
         <v>42395</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="63" t="s">
+      <c r="A71" s="73" t="s">
         <v>110</v>
       </c>
-      <c r="B71" s="64"/>
-      <c r="C71" s="64"/>
-      <c r="D71" s="64"/>
-      <c r="E71" s="64"/>
-      <c r="F71" s="64"/>
-      <c r="G71" s="64"/>
-      <c r="H71" s="65"/>
+      <c r="B71" s="74"/>
+      <c r="C71" s="74"/>
+      <c r="D71" s="74"/>
+      <c r="E71" s="74"/>
+      <c r="F71" s="74"/>
+      <c r="G71" s="74"/>
+      <c r="H71" s="75"/>
     </row>
     <row r="72" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A72" s="18">
@@ -2790,7 +2790,7 @@
       <c r="G72" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="H72" s="67">
+      <c r="H72" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2814,7 +2814,7 @@
       <c r="G73" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="H73" s="67">
+      <c r="H73" s="63">
         <v>42395</v>
       </c>
     </row>
@@ -2838,21 +2838,21 @@
       <c r="G74" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="H74" s="67">
+      <c r="H74" s="63">
         <v>42395</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="63" t="s">
+      <c r="A75" s="73" t="s">
         <v>116</v>
       </c>
-      <c r="B75" s="70"/>
-      <c r="C75" s="70"/>
-      <c r="D75" s="70"/>
-      <c r="E75" s="64"/>
-      <c r="F75" s="64"/>
-      <c r="G75" s="64"/>
-      <c r="H75" s="65"/>
+      <c r="B75" s="76"/>
+      <c r="C75" s="76"/>
+      <c r="D75" s="76"/>
+      <c r="E75" s="74"/>
+      <c r="F75" s="74"/>
+      <c r="G75" s="74"/>
+      <c r="H75" s="75"/>
     </row>
     <row r="76" spans="1:8" ht="75" x14ac:dyDescent="0.25">
       <c r="A76" s="44">
@@ -2865,64 +2865,64 @@
         <v>119</v>
       </c>
       <c r="D76" s="38"/>
-      <c r="E76" s="69" t="s">
+      <c r="E76" s="65" t="s">
         <v>120</v>
       </c>
-      <c r="F76" s="71" t="s">
-        <v>127</v>
+      <c r="F76" s="66" t="s">
+        <v>126</v>
       </c>
       <c r="G76" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="H76" s="72">
+      <c r="H76" s="67">
         <v>42401</v>
       </c>
     </row>
-    <row r="77" spans="1:8" ht="90" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A77" s="18">
         <v>65</v>
       </c>
-      <c r="B77" s="74" t="s">
+      <c r="B77" s="69" t="s">
         <v>118</v>
       </c>
-      <c r="C77" s="74" t="s">
+      <c r="C77" s="69" t="s">
         <v>121</v>
       </c>
-      <c r="D77" s="74"/>
-      <c r="E77" s="75" t="s">
+      <c r="D77" s="69"/>
+      <c r="E77" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="F77" s="76" t="s">
-        <v>128</v>
-      </c>
-      <c r="G77" s="75" t="s">
+      <c r="F77" s="71" t="s">
+        <v>127</v>
+      </c>
+      <c r="G77" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="H77" s="77">
+      <c r="H77" s="72">
         <v>42401</v>
       </c>
     </row>
-    <row r="78" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A78" s="18">
         <v>66</v>
       </c>
       <c r="B78" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="C78" s="53" t="s">
         <v>123</v>
-      </c>
-      <c r="C78" s="53" t="s">
-        <v>124</v>
       </c>
       <c r="D78" s="53"/>
       <c r="E78" s="53" t="s">
+        <v>124</v>
+      </c>
+      <c r="F78" s="56" t="s">
         <v>125</v>
-      </c>
-      <c r="F78" s="56" t="s">
-        <v>126</v>
       </c>
       <c r="G78" s="53" t="s">
         <v>74</v>
       </c>
-      <c r="H78" s="72">
+      <c r="H78" s="67">
         <v>42401</v>
       </c>
     </row>
@@ -2987,16 +2987,16 @@
       <c r="H83" s="61"/>
     </row>
     <row r="84" spans="1:8" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="63" t="s">
+      <c r="A84" s="73" t="s">
         <v>109</v>
       </c>
-      <c r="B84" s="64"/>
-      <c r="C84" s="64"/>
-      <c r="D84" s="64"/>
-      <c r="E84" s="64"/>
-      <c r="F84" s="64"/>
-      <c r="G84" s="64"/>
-      <c r="H84" s="65"/>
+      <c r="B84" s="74"/>
+      <c r="C84" s="74"/>
+      <c r="D84" s="74"/>
+      <c r="E84" s="74"/>
+      <c r="F84" s="74"/>
+      <c r="G84" s="74"/>
+      <c r="H84" s="75"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="18"/>
@@ -3076,7 +3076,7 @@
       <c r="E92" s="38"/>
       <c r="F92" s="45"/>
       <c r="G92" s="38"/>
-      <c r="H92" s="68"/>
+      <c r="H92" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>